<commit_message>
A typo on file name is fixed.
</commit_message>
<xml_diff>
--- a/columns.xlsx
+++ b/columns.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">columns!$A$1:$C$105</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
   <si>
     <t>Id</t>
   </si>
@@ -856,12 +859,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -874,6 +874,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1229,857 +1231,873 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4"/>
+    <col min="4" max="4" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="5"/>
+    </row>
+    <row r="57" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="60" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="5"/>
     </row>
     <row r="61" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="5"/>
     </row>
     <row r="62" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="5"/>
     </row>
     <row r="64" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="5"/>
     </row>
     <row r="65" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="5"/>
     </row>
     <row r="66" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="5"/>
     </row>
     <row r="69" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="5"/>
     </row>
     <row r="70" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>68</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="5"/>
     </row>
     <row r="71" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="5"/>
     </row>
     <row r="72" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="5"/>
+    </row>
+    <row r="73" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="75" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="77" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>75</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="5"/>
     </row>
     <row r="78" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="5"/>
     </row>
     <row r="79" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
-      </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="5"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C81" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
-      </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="2"/>
+      <c r="C84" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D84"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="5"/>
       <c r="D85"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
-      </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="5"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D90"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="3"/>
-      <c r="C91" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="5"/>
       <c r="D91"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="6"/>
       <c r="D92"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="5"/>
       <c r="D93"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>92</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" s="5"/>
       <c r="D94"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D95"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D96"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>95</v>
-      </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D97"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>96</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="5"/>
       <c r="D98"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>97</v>
-      </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D99"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>98</v>
-      </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" s="5"/>
       <c r="D100"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101" s="5"/>
       <c r="D101"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>100</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="5"/>
       <c r="D102"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>101</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="C103" s="5"/>
       <c r="D103"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>102</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B104" s="2"/>
+      <c r="C104" s="5"/>
       <c r="D104"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>103</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="5"/>
       <c r="D105"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B81:C81"/>
-  </mergeCells>
+  <autoFilter ref="A1:C105" xr:uid="{DB4C1184-FD31-4676-92A4-0D6751343846}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+    <sortState ref="A2:C105">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates on feature engineering.
</commit_message>
<xml_diff>
--- a/columns.xlsx
+++ b/columns.xlsx
@@ -15,14 +15,14 @@
     <sheet name="columns" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">columns!$A$1:$C$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">columns!$A$1:$E$102</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="112">
   <si>
     <t>Id</t>
   </si>
@@ -273,9 +273,6 @@
     <t>logSP</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -285,33 +282,6 @@
     <t>Story</t>
   </si>
   <si>
-    <t>Artery</t>
-  </si>
-  <si>
-    <t>Feedr</t>
-  </si>
-  <si>
-    <t>RRNn</t>
-  </si>
-  <si>
-    <t>RRAn</t>
-  </si>
-  <si>
-    <t>PosN</t>
-  </si>
-  <si>
-    <t>PosA</t>
-  </si>
-  <si>
-    <t>RRNe</t>
-  </si>
-  <si>
-    <t>RRAe</t>
-  </si>
-  <si>
-    <t>Norm</t>
-  </si>
-  <si>
     <t>DoubleExterior</t>
   </si>
   <si>
@@ -346,6 +316,48 @@
   </si>
   <si>
     <t>No Need</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>PossibleVar</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Dependent</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>RemodeledAge</t>
+  </si>
+  <si>
+    <t>RemodeledAge2</t>
+  </si>
+  <si>
+    <t>FurtherNotes</t>
+  </si>
+  <si>
+    <t>Will be used in an indirect way for predictions.</t>
+  </si>
+  <si>
+    <t>TotalPorchSF</t>
+  </si>
+  <si>
+    <t>OneKitchen</t>
+  </si>
+  <si>
+    <t>Proximity</t>
   </si>
 </sst>
 </file>
@@ -875,7 +887,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1231,871 +1245,1155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="3"/>
+    <col min="2" max="2" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1"/>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D36" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D44" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D45" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D47" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B48" s="2"/>
       <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D53" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D54" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" s="5"/>
-    </row>
-    <row r="56" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C57" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D60" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D62" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D63" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D64" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>25</v>
-      </c>
-      <c r="B65" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D65" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D66" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>73</v>
-      </c>
-      <c r="B67" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D67" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C68" s="5"/>
-    </row>
-    <row r="69" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D68" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>75</v>
-      </c>
-      <c r="B69" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C69" s="5"/>
-    </row>
-    <row r="70" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D69" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C70" s="5"/>
-    </row>
-    <row r="71" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D70" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C71" s="5"/>
-    </row>
-    <row r="72" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" s="5"/>
-    </row>
-    <row r="73" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>66</v>
-      </c>
-      <c r="B75" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D75" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>102</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C77" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D78" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>71</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="5"/>
-      <c r="D81"/>
-    </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>92</v>
-      </c>
-      <c r="B82" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C82" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>106</v>
       </c>
-      <c r="D82"/>
-    </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="2"/>
+      <c r="B83" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C83" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D83"/>
-    </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D84"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="5"/>
-      <c r="D85"/>
+      <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="5"/>
-      <c r="D86"/>
-    </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D87"/>
-    </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B88" s="2"/>
-      <c r="C88" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D88"/>
-    </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C88" s="5"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>93</v>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D89"/>
-    </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D90"/>
+        <v>96</v>
+      </c>
+      <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B91" s="2"/>
-      <c r="C91" s="5"/>
-      <c r="D91"/>
+      <c r="C91" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>79</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C92" s="6"/>
-      <c r="D92"/>
+        <v>85</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>77</v>
-      </c>
-      <c r="B93" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C93" s="5"/>
-      <c r="D93"/>
+      <c r="D93" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B94" s="2"/>
-      <c r="C94" s="5"/>
-      <c r="D94"/>
-    </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C94" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>97</v>
-      </c>
-      <c r="B95" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C95" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D95"/>
-    </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>101</v>
-      </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D96"/>
-    </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>86</v>
-      </c>
-      <c r="B97" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C97" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D97"/>
+        <v>96</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C98" s="5"/>
-      <c r="D98"/>
-    </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="D98" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>100</v>
-      </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D99"/>
+        <v>65</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>37</v>
-      </c>
-      <c r="B100" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C100" s="5"/>
-      <c r="D100"/>
+      <c r="D100" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>53</v>
-      </c>
-      <c r="B101" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C101" s="5"/>
-      <c r="D101"/>
+      <c r="D101" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>65</v>
-      </c>
-      <c r="B102" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C102" s="5"/>
-      <c r="D102"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>18</v>
-      </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="5"/>
-      <c r="D103"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>19</v>
-      </c>
-      <c r="B104" s="2"/>
-      <c r="C104" s="5"/>
-      <c r="D104"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>76</v>
-      </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="5"/>
-      <c r="D105"/>
+      <c r="D102" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C105" xr:uid="{DB4C1184-FD31-4676-92A4-0D6751343846}">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-    <sortState ref="A2:C105">
-      <sortCondition ref="A1"/>
+  <autoFilter ref="A1:E102" xr:uid="{3467CDFD-EAC6-4C83-B6B6-33FD9C199EDC}">
+    <sortState ref="A2:E102">
+      <sortCondition ref="A1:A102"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Theme update on Plots
</commit_message>
<xml_diff>
--- a/columns.xlsx
+++ b/columns.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazimanil\Documents\R_Projects\House_Prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Documents\R_Projects\House_Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="113">
   <si>
     <t>Id</t>
   </si>
@@ -358,12 +358,15 @@
   </si>
   <si>
     <t>Proximity</t>
+  </si>
+  <si>
+    <t>PoolQC will be used instead</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1244,11 +1247,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1365,7 +1368,9 @@
       <c r="C9" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1375,7 +1380,9 @@
       <c r="C10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1533,7 +1540,9 @@
       <c r="C25" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2036,7 +2045,9 @@
       <c r="C71" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -2072,7 +2083,9 @@
       <c r="C74" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D74" s="2"/>
+      <c r="D74" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -2119,16 +2132,23 @@
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="E78" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>71</v>
       </c>
-      <c r="B79" s="2"/>
+      <c r="B79" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C79" s="5"/>
-      <c r="D79" s="2"/>
+      <c r="D79" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
@@ -2152,7 +2172,9 @@
       <c r="C81" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
@@ -2246,7 +2268,9 @@
       <c r="C90" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D90" s="2"/>
+      <c r="D90" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
@@ -2256,7 +2280,9 @@
       <c r="C91" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D91" s="2"/>
+      <c r="D91" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
@@ -2266,7 +2292,9 @@
       <c r="C92" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D92" s="2"/>
+      <c r="D92" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
@@ -2288,7 +2316,9 @@
       <c r="C94" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
@@ -2391,7 +2421,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E102" xr:uid="{3467CDFD-EAC6-4C83-B6B6-33FD9C199EDC}">
+  <autoFilter ref="A1:E102">
     <sortState ref="A2:E102">
       <sortCondition ref="A1:A102"/>
     </sortState>

</xml_diff>

<commit_message>
Latest advances on Data Munging.
</commit_message>
<xml_diff>
--- a/columns.xlsx
+++ b/columns.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Documents\R_Projects\House_Prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazimanil\Documents\R_Projects\House_Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">columns!$A$1:$E$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">columns!$A$1:$E$104</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="117">
   <si>
     <t>Id</t>
   </si>
@@ -361,12 +361,24 @@
   </si>
   <si>
     <t>PoolQC will be used instead</t>
+  </si>
+  <si>
+    <t>GarageArea will be used instead</t>
+  </si>
+  <si>
+    <t>GoodFinBsmt</t>
+  </si>
+  <si>
+    <t>NewBuilding</t>
+  </si>
+  <si>
+    <t>should be checked with Story &amp; Age variables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1247,11 +1259,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1278,7 +1291,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1290,7 +1303,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1302,7 +1315,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1314,7 +1327,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1356,9 +1369,13 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1384,23 +1401,31 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1412,7 +1437,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1424,25 +1449,33 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>96</v>
@@ -1452,9 +1485,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>96</v>
@@ -1464,17 +1497,21 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>29</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>96</v>
@@ -1484,33 +1521,39 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>96</v>
@@ -1519,22 +1562,28 @@
       <c r="D23" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>93</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>86</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="5" t="s">
@@ -1544,41 +1593,45 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>41</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>27</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>96</v>
@@ -1588,9 +1641,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>96</v>
@@ -1600,297 +1653,357 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>56</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>28</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>48</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>54</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>61</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>57</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>58</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B50" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="C51" s="6"/>
+      <c r="D51" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="B52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>52</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>8</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>81</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>82</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>4</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>9</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>96</v>
@@ -1900,9 +2013,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>96</v>
@@ -1912,47 +2025,47 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="5"/>
+      <c r="D61" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B62" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>44</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>25</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>96</v>
@@ -1964,46 +2077,46 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>96</v>
@@ -2013,21 +2126,21 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>96</v>
@@ -2039,23 +2152,21 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="5" t="s">
-        <v>96</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="5"/>
       <c r="D71" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B72" s="2"/>
       <c r="C72" s="5" t="s">
         <v>96</v>
       </c>
@@ -2065,134 +2176,134 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>66</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>92</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="B74" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="5"/>
       <c r="D74" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>17</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>16</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="5" t="s">
-        <v>96</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" s="5"/>
       <c r="D77" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>64</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>70</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E78" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>71</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="E79" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="C80" s="5"/>
       <c r="D80" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>105</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="B82" s="2"/>
       <c r="C82" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>96</v>
@@ -2206,87 +2317,105 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>21</v>
       </c>
-      <c r="B84" s="2"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" s="2"/>
+      <c r="B85" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C85" s="5"/>
-      <c r="D85" s="2"/>
+      <c r="D85" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>78</v>
       </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>79</v>
-      </c>
       <c r="B87" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>77</v>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>115</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>69</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90" s="2"/>
-      <c r="C90" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" s="2"/>
-      <c r="C91" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="B91" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C91" s="5"/>
       <c r="D91" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="5" t="s">
@@ -2298,19 +2427,19 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C93" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="D93" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="5" t="s">
@@ -2320,35 +2449,33 @@
         <v>101</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="C95" s="5"/>
       <c r="D95" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>37</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="D96" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>96</v>
@@ -2362,68 +2489,99 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="5"/>
+      <c r="C99" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="D99" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>76</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="2" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E102">
-    <sortState ref="A2:E102">
-      <sortCondition ref="A1:A102"/>
+  <autoFilter ref="A1:E104" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="YES"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:E104">
+      <sortCondition ref="A1:A104"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
XG Boost predictions submitted.
</commit_message>
<xml_diff>
--- a/columns.xlsx
+++ b/columns.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="117">
   <si>
     <t>Id</t>
   </si>
@@ -1263,8 +1263,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1547,9 +1547,6 @@
       <c r="D22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">

</xml_diff>